<commit_message>
New plots and functios predicted vs observed
</commit_message>
<xml_diff>
--- a/data-raw/dataEntryTemplateCalfSim.xlsx
+++ b/data-raw/dataEntryTemplateCalfSim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadeu\OneDrive\Documentos\Postdoc - UVM\CalfSim\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33671331-CDE7-47A8-A571-6469B7548D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF494C8-5181-47DE-A502-51FBBCC9D89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{36B5F550-BD63-4E1F-A7FD-DBBA2246A2ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>animal</t>
   </si>
@@ -44,13 +44,19 @@
     <t>age_days</t>
   </si>
   <si>
-    <t>weight_kg</t>
+    <t>birth_weight_kg</t>
+  </si>
+  <si>
+    <t>body_weight_kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,27 +403,932 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BA3463-CB4F-4EC1-83A4-0183233DD4D8}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>44.8</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>80.679999999999993</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="C3">
+        <v>61</v>
+      </c>
+      <c r="D3">
+        <v>61.221000000000004</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>71.259999999999991</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>42.5</v>
+      </c>
+      <c r="C5">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>73.905000000000001</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>44.6</v>
+      </c>
+      <c r="C6">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>70.093000000000004</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>44.4</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+      <c r="D7">
+        <v>69.644999999999996</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>35.9</v>
+      </c>
+      <c r="C8">
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <v>60.385999999999996</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="C9">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>72.954000000000008</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C10">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>52.524999999999999</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>35.9</v>
+      </c>
+      <c r="C11">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>66.027999999999992</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>42.9</v>
+      </c>
+      <c r="C12">
+        <v>53</v>
+      </c>
+      <c r="D12">
+        <v>61.661999999999999</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>40.6</v>
+      </c>
+      <c r="C13">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>66.198999999999998</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>40.1</v>
+      </c>
+      <c r="C14">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <v>68.31</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>42.4</v>
+      </c>
+      <c r="C15">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <v>72.364999999999995</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>42.4</v>
+      </c>
+      <c r="C16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>72.135999999999996</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>43.3</v>
+      </c>
+      <c r="C17">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>63.225999999999999</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>42.5</v>
+      </c>
+      <c r="C18">
+        <v>62</v>
+      </c>
+      <c r="D18">
+        <v>78.77</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>43.6</v>
+      </c>
+      <c r="C19">
+        <v>55</v>
+      </c>
+      <c r="D19">
+        <v>68.295000000000002</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>37.1</v>
+      </c>
+      <c r="C20">
+        <v>52</v>
+      </c>
+      <c r="D20">
+        <v>69.807999999999993</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21">
+        <v>64.34</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>44.2</v>
+      </c>
+      <c r="C22">
+        <v>65</v>
+      </c>
+      <c r="D22">
+        <v>79.754999999999995</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>41.2</v>
+      </c>
+      <c r="C23">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>68.528000000000006</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>43.3</v>
+      </c>
+      <c r="C24">
+        <v>54</v>
+      </c>
+      <c r="D24">
+        <v>74.349999999999994</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>43.1</v>
+      </c>
+      <c r="C25">
+        <v>65</v>
+      </c>
+      <c r="D25">
+        <v>73.844999999999999</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="C26">
+        <v>55</v>
+      </c>
+      <c r="D26">
+        <v>65.11</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="C27">
+        <v>51</v>
+      </c>
+      <c r="D27">
+        <v>56.070000000000007</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>40.4</v>
+      </c>
+      <c r="C28">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>69.664000000000001</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>37.4</v>
+      </c>
+      <c r="C29">
+        <v>63</v>
+      </c>
+      <c r="D29">
+        <v>64.805000000000007</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>53</v>
+      </c>
+      <c r="D30">
+        <v>52.861000000000004</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>42.6</v>
+      </c>
+      <c r="C31">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>69</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="C32">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>64.2</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="C33">
+        <v>57</v>
+      </c>
+      <c r="D33">
+        <v>52.870000000000005</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>43.1</v>
+      </c>
+      <c r="C34">
+        <v>61</v>
+      </c>
+      <c r="D34">
+        <v>68.231999999999999</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>44.1</v>
+      </c>
+      <c r="C35">
+        <v>57</v>
+      </c>
+      <c r="D35">
+        <v>80.751000000000005</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="C36">
+        <v>59</v>
+      </c>
+      <c r="D36">
+        <v>70.983000000000004</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="C37">
+        <v>53</v>
+      </c>
+      <c r="D37">
+        <v>72.12299999999999</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <v>62.239999999999995</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>54</v>
+      </c>
+      <c r="D39">
+        <v>66.460000000000008</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>41.2</v>
+      </c>
+      <c r="C40">
+        <v>58</v>
+      </c>
+      <c r="D40">
+        <v>68.807999999999993</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>44.6</v>
+      </c>
+      <c r="C41">
+        <v>60</v>
+      </c>
+      <c r="D41">
+        <v>71.84</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>36.4</v>
+      </c>
+      <c r="C42">
+        <v>51</v>
+      </c>
+      <c r="D42">
+        <v>53.841999999999999</v>
+      </c>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>41.1</v>
+      </c>
+      <c r="C43">
+        <v>56</v>
+      </c>
+      <c r="D43">
+        <v>74.307999999999993</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>44.1</v>
+      </c>
+      <c r="C44">
+        <v>63</v>
+      </c>
+      <c r="D44">
+        <v>70.245000000000005</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>36.6</v>
+      </c>
+      <c r="C45">
+        <v>53</v>
+      </c>
+      <c r="D45">
+        <v>70.52000000000001</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>42.4</v>
+      </c>
+      <c r="C46">
+        <v>63</v>
+      </c>
+      <c r="D46">
+        <v>80.578000000000003</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="C47">
+        <v>54</v>
+      </c>
+      <c r="D47">
+        <v>62.951999999999998</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>41.1</v>
+      </c>
+      <c r="C48">
+        <v>51</v>
+      </c>
+      <c r="D48">
+        <v>70.730999999999995</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>41.6</v>
+      </c>
+      <c r="C49">
+        <v>62</v>
+      </c>
+      <c r="D49">
+        <v>70.739999999999995</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>41.9</v>
+      </c>
+      <c r="C50">
+        <v>66</v>
+      </c>
+      <c r="D50">
+        <v>61.963999999999999</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="C51">
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <v>68.36</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>